<commit_message>
[PM-498] Add importer and exporter for FC
</commit_message>
<xml_diff>
--- a/spec/fixtures/expected_program_spreadsheet.xlsx
+++ b/spec/fixtures/expected_program_spreadsheet.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selks\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB64377-04B4-3843-B331-791D09F1FE48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="11388"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15760" windowHeight="11380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
+    <sheet name="Funding Contributors" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
@@ -90,22 +92,28 @@
     <definedName name="wages_freq_int_rec" localSheetId="0">#REF!</definedName>
     <definedName name="wages_freq_int_rec">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Registered User</author>
   </authors>
   <commentList>
-    <comment ref="CD6" authorId="0" shapeId="0">
+    <comment ref="CD6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1485,13 +1493,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1817,7 +1825,7 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -1891,7 +1899,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1911,22 +1919,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1935,10 +1943,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1992,7 +2000,7 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2000,37 +2008,31 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2063,41 +2065,47 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="%" xfId="3"/>
-    <cellStyle name="% 2 2 2" xfId="4"/>
+    <cellStyle name="%" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% 2 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8"/>
-    <cellStyle name="Normal 2 2" xfId="6"/>
-    <cellStyle name="Normal_RCP" xfId="5"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Percent 11" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2486,14 +2494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:KL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
@@ -2501,9 +2509,9 @@
       <selection pane="bottomRight" activeCell="KL18" sqref="KL18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" style="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="6" width="21" style="1" customWidth="1"/>
@@ -2521,17 +2529,17 @@
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
     <col min="279" max="285" width="21" style="29" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
-    <col min="294" max="296" width="22.1796875" style="7" customWidth="1"/>
-    <col min="297" max="297" width="13.1796875" style="7" customWidth="1"/>
+    <col min="294" max="296" width="22.140625" style="7" customWidth="1"/>
+    <col min="297" max="297" width="13.140625" style="7" customWidth="1"/>
     <col min="298" max="298" width="11" style="7" customWidth="1"/>
-    <col min="299" max="16384" width="8.81640625" style="7"/>
+    <col min="299" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="62"/>
+    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2824,11 +2832,11 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="82" t="s">
         <v>320</v>
       </c>
-      <c r="B2" s="63"/>
+      <c r="B2" s="82"/>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
       <c r="E2" s="23"/>
@@ -3121,7 +3129,7 @@
       <c r="KF2" s="42"/>
       <c r="KG2" s="42"/>
     </row>
-    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="44"/>
@@ -3416,423 +3424,423 @@
       <c r="KF3" s="50"/>
       <c r="KG3" s="50"/>
     </row>
-    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65" t="s">
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="66" t="s">
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="67" t="s">
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68" t="s">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="68"/>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68"/>
-      <c r="AC4" s="69" t="s">
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="69"/>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="69"/>
-      <c r="AG4" s="69"/>
-      <c r="AH4" s="69"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="70" t="s">
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="70"/>
-      <c r="AL4" s="70"/>
-      <c r="AM4" s="61" t="s">
+      <c r="AK4" s="89"/>
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="73" t="s">
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="70"/>
+      <c r="AQ4" s="70"/>
+      <c r="AR4" s="70"/>
+      <c r="AS4" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="73"/>
-      <c r="AY4" s="73"/>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="73"/>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="73"/>
-      <c r="BF4" s="73"/>
-      <c r="BG4" s="73"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="71" t="s">
+      <c r="AT4" s="71"/>
+      <c r="AU4" s="71"/>
+      <c r="AV4" s="71"/>
+      <c r="AW4" s="71"/>
+      <c r="AX4" s="71"/>
+      <c r="AY4" s="71"/>
+      <c r="AZ4" s="71"/>
+      <c r="BA4" s="71"/>
+      <c r="BB4" s="71"/>
+      <c r="BC4" s="71"/>
+      <c r="BD4" s="71"/>
+      <c r="BE4" s="71"/>
+      <c r="BF4" s="71"/>
+      <c r="BG4" s="71"/>
+      <c r="BH4" s="71"/>
+      <c r="BI4" s="71"/>
+      <c r="BJ4" s="71"/>
+      <c r="BK4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="71"/>
-      <c r="BM4" s="71"/>
-      <c r="BN4" s="71"/>
-      <c r="BO4" s="71"/>
-      <c r="BP4" s="71"/>
-      <c r="BQ4" s="71"/>
-      <c r="BR4" s="71"/>
-      <c r="BS4" s="71"/>
-      <c r="BT4" s="71"/>
-      <c r="BU4" s="71"/>
-      <c r="BV4" s="71"/>
-      <c r="BW4" s="71"/>
-      <c r="BX4" s="71"/>
-      <c r="BY4" s="74" t="s">
+      <c r="BL4" s="67"/>
+      <c r="BM4" s="67"/>
+      <c r="BN4" s="67"/>
+      <c r="BO4" s="67"/>
+      <c r="BP4" s="67"/>
+      <c r="BQ4" s="67"/>
+      <c r="BR4" s="67"/>
+      <c r="BS4" s="67"/>
+      <c r="BT4" s="67"/>
+      <c r="BU4" s="67"/>
+      <c r="BV4" s="67"/>
+      <c r="BW4" s="67"/>
+      <c r="BX4" s="67"/>
+      <c r="BY4" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="74"/>
-      <c r="CA4" s="74"/>
-      <c r="CB4" s="74"/>
-      <c r="CC4" s="74"/>
-      <c r="CD4" s="74"/>
-      <c r="CE4" s="74"/>
-      <c r="CF4" s="74"/>
-      <c r="CG4" s="74"/>
-      <c r="CH4" s="74"/>
-      <c r="CI4" s="74"/>
-      <c r="CJ4" s="74"/>
-      <c r="CK4" s="74"/>
-      <c r="CL4" s="74"/>
-      <c r="CM4" s="75" t="s">
+      <c r="BZ4" s="72"/>
+      <c r="CA4" s="72"/>
+      <c r="CB4" s="72"/>
+      <c r="CC4" s="72"/>
+      <c r="CD4" s="72"/>
+      <c r="CE4" s="72"/>
+      <c r="CF4" s="72"/>
+      <c r="CG4" s="72"/>
+      <c r="CH4" s="72"/>
+      <c r="CI4" s="72"/>
+      <c r="CJ4" s="72"/>
+      <c r="CK4" s="72"/>
+      <c r="CL4" s="72"/>
+      <c r="CM4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="75"/>
-      <c r="CO4" s="75"/>
-      <c r="CP4" s="75"/>
-      <c r="CQ4" s="75"/>
-      <c r="CR4" s="75"/>
-      <c r="CS4" s="75"/>
-      <c r="CT4" s="75"/>
-      <c r="CU4" s="75"/>
-      <c r="CV4" s="75"/>
-      <c r="CW4" s="75"/>
-      <c r="CX4" s="75"/>
-      <c r="CY4" s="75"/>
-      <c r="CZ4" s="75"/>
-      <c r="DA4" s="76" t="s">
+      <c r="CN4" s="73"/>
+      <c r="CO4" s="73"/>
+      <c r="CP4" s="73"/>
+      <c r="CQ4" s="73"/>
+      <c r="CR4" s="73"/>
+      <c r="CS4" s="73"/>
+      <c r="CT4" s="73"/>
+      <c r="CU4" s="73"/>
+      <c r="CV4" s="73"/>
+      <c r="CW4" s="73"/>
+      <c r="CX4" s="73"/>
+      <c r="CY4" s="73"/>
+      <c r="CZ4" s="73"/>
+      <c r="DA4" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="76"/>
-      <c r="DC4" s="76"/>
-      <c r="DD4" s="76"/>
-      <c r="DE4" s="76"/>
-      <c r="DF4" s="76"/>
-      <c r="DG4" s="76"/>
-      <c r="DH4" s="76"/>
-      <c r="DI4" s="76"/>
-      <c r="DJ4" s="76"/>
-      <c r="DK4" s="76"/>
-      <c r="DL4" s="76"/>
-      <c r="DM4" s="76"/>
-      <c r="DN4" s="76"/>
-      <c r="DO4" s="77" t="s">
+      <c r="DB4" s="74"/>
+      <c r="DC4" s="74"/>
+      <c r="DD4" s="74"/>
+      <c r="DE4" s="74"/>
+      <c r="DF4" s="74"/>
+      <c r="DG4" s="74"/>
+      <c r="DH4" s="74"/>
+      <c r="DI4" s="74"/>
+      <c r="DJ4" s="74"/>
+      <c r="DK4" s="74"/>
+      <c r="DL4" s="74"/>
+      <c r="DM4" s="74"/>
+      <c r="DN4" s="74"/>
+      <c r="DO4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="77"/>
-      <c r="DQ4" s="77"/>
-      <c r="DR4" s="77"/>
-      <c r="DS4" s="77"/>
-      <c r="DT4" s="77"/>
-      <c r="DU4" s="77"/>
-      <c r="DV4" s="77"/>
-      <c r="DW4" s="77"/>
-      <c r="DX4" s="77"/>
-      <c r="DY4" s="77"/>
-      <c r="DZ4" s="77"/>
-      <c r="EA4" s="77"/>
-      <c r="EB4" s="77"/>
-      <c r="EC4" s="78" t="s">
+      <c r="DP4" s="75"/>
+      <c r="DQ4" s="75"/>
+      <c r="DR4" s="75"/>
+      <c r="DS4" s="75"/>
+      <c r="DT4" s="75"/>
+      <c r="DU4" s="75"/>
+      <c r="DV4" s="75"/>
+      <c r="DW4" s="75"/>
+      <c r="DX4" s="75"/>
+      <c r="DY4" s="75"/>
+      <c r="DZ4" s="75"/>
+      <c r="EA4" s="75"/>
+      <c r="EB4" s="75"/>
+      <c r="EC4" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="78"/>
-      <c r="EE4" s="78"/>
-      <c r="EF4" s="78"/>
-      <c r="EG4" s="78"/>
-      <c r="EH4" s="78"/>
-      <c r="EI4" s="78"/>
-      <c r="EJ4" s="78"/>
-      <c r="EK4" s="78"/>
-      <c r="EL4" s="78"/>
-      <c r="EM4" s="78"/>
-      <c r="EN4" s="78"/>
-      <c r="EO4" s="78"/>
-      <c r="EP4" s="78"/>
-      <c r="EQ4" s="79" t="s">
+      <c r="ED4" s="76"/>
+      <c r="EE4" s="76"/>
+      <c r="EF4" s="76"/>
+      <c r="EG4" s="76"/>
+      <c r="EH4" s="76"/>
+      <c r="EI4" s="76"/>
+      <c r="EJ4" s="76"/>
+      <c r="EK4" s="76"/>
+      <c r="EL4" s="76"/>
+      <c r="EM4" s="76"/>
+      <c r="EN4" s="76"/>
+      <c r="EO4" s="76"/>
+      <c r="EP4" s="76"/>
+      <c r="EQ4" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="79"/>
-      <c r="ES4" s="79"/>
-      <c r="ET4" s="79"/>
-      <c r="EU4" s="79"/>
-      <c r="EV4" s="79"/>
-      <c r="EW4" s="79"/>
-      <c r="EX4" s="79"/>
-      <c r="EY4" s="79"/>
-      <c r="EZ4" s="79"/>
-      <c r="FA4" s="79"/>
-      <c r="FB4" s="79"/>
-      <c r="FC4" s="79"/>
-      <c r="FD4" s="79"/>
-      <c r="FE4" s="80" t="s">
+      <c r="ER4" s="77"/>
+      <c r="ES4" s="77"/>
+      <c r="ET4" s="77"/>
+      <c r="EU4" s="77"/>
+      <c r="EV4" s="77"/>
+      <c r="EW4" s="77"/>
+      <c r="EX4" s="77"/>
+      <c r="EY4" s="77"/>
+      <c r="EZ4" s="77"/>
+      <c r="FA4" s="77"/>
+      <c r="FB4" s="77"/>
+      <c r="FC4" s="77"/>
+      <c r="FD4" s="77"/>
+      <c r="FE4" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="80"/>
-      <c r="FG4" s="80"/>
-      <c r="FH4" s="80"/>
-      <c r="FI4" s="80"/>
-      <c r="FJ4" s="80"/>
-      <c r="FK4" s="80"/>
-      <c r="FL4" s="80"/>
-      <c r="FM4" s="80"/>
-      <c r="FN4" s="80"/>
-      <c r="FO4" s="80"/>
-      <c r="FP4" s="80"/>
-      <c r="FQ4" s="80"/>
-      <c r="FR4" s="80"/>
-      <c r="FS4" s="81" t="s">
+      <c r="FF4" s="78"/>
+      <c r="FG4" s="78"/>
+      <c r="FH4" s="78"/>
+      <c r="FI4" s="78"/>
+      <c r="FJ4" s="78"/>
+      <c r="FK4" s="78"/>
+      <c r="FL4" s="78"/>
+      <c r="FM4" s="78"/>
+      <c r="FN4" s="78"/>
+      <c r="FO4" s="78"/>
+      <c r="FP4" s="78"/>
+      <c r="FQ4" s="78"/>
+      <c r="FR4" s="78"/>
+      <c r="FS4" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="81"/>
-      <c r="FU4" s="81"/>
-      <c r="FV4" s="81"/>
-      <c r="FW4" s="81"/>
-      <c r="FX4" s="81"/>
-      <c r="FY4" s="81"/>
-      <c r="FZ4" s="81"/>
-      <c r="GA4" s="81"/>
-      <c r="GB4" s="81"/>
-      <c r="GC4" s="81"/>
-      <c r="GD4" s="81"/>
-      <c r="GE4" s="81"/>
-      <c r="GF4" s="81"/>
-      <c r="GG4" s="71" t="s">
+      <c r="FT4" s="79"/>
+      <c r="FU4" s="79"/>
+      <c r="FV4" s="79"/>
+      <c r="FW4" s="79"/>
+      <c r="FX4" s="79"/>
+      <c r="FY4" s="79"/>
+      <c r="FZ4" s="79"/>
+      <c r="GA4" s="79"/>
+      <c r="GB4" s="79"/>
+      <c r="GC4" s="79"/>
+      <c r="GD4" s="79"/>
+      <c r="GE4" s="79"/>
+      <c r="GF4" s="79"/>
+      <c r="GG4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="71"/>
-      <c r="GI4" s="71"/>
-      <c r="GJ4" s="71"/>
-      <c r="GK4" s="71"/>
-      <c r="GL4" s="71"/>
-      <c r="GM4" s="71"/>
-      <c r="GN4" s="71"/>
-      <c r="GO4" s="71"/>
-      <c r="GP4" s="71"/>
-      <c r="GQ4" s="71"/>
-      <c r="GR4" s="71"/>
-      <c r="GS4" s="71"/>
-      <c r="GT4" s="71"/>
-      <c r="GU4" s="71" t="s">
+      <c r="GH4" s="67"/>
+      <c r="GI4" s="67"/>
+      <c r="GJ4" s="67"/>
+      <c r="GK4" s="67"/>
+      <c r="GL4" s="67"/>
+      <c r="GM4" s="67"/>
+      <c r="GN4" s="67"/>
+      <c r="GO4" s="67"/>
+      <c r="GP4" s="67"/>
+      <c r="GQ4" s="67"/>
+      <c r="GR4" s="67"/>
+      <c r="GS4" s="67"/>
+      <c r="GT4" s="67"/>
+      <c r="GU4" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="71"/>
-      <c r="GW4" s="71"/>
-      <c r="GX4" s="71"/>
-      <c r="GY4" s="71"/>
-      <c r="GZ4" s="71"/>
-      <c r="HA4" s="71"/>
-      <c r="HB4" s="71"/>
-      <c r="HC4" s="71"/>
-      <c r="HD4" s="71"/>
-      <c r="HE4" s="71"/>
-      <c r="HF4" s="71"/>
-      <c r="HG4" s="71"/>
-      <c r="HH4" s="71"/>
-      <c r="HI4" s="71" t="s">
+      <c r="GV4" s="67"/>
+      <c r="GW4" s="67"/>
+      <c r="GX4" s="67"/>
+      <c r="GY4" s="67"/>
+      <c r="GZ4" s="67"/>
+      <c r="HA4" s="67"/>
+      <c r="HB4" s="67"/>
+      <c r="HC4" s="67"/>
+      <c r="HD4" s="67"/>
+      <c r="HE4" s="67"/>
+      <c r="HF4" s="67"/>
+      <c r="HG4" s="67"/>
+      <c r="HH4" s="67"/>
+      <c r="HI4" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="71"/>
-      <c r="HK4" s="71"/>
-      <c r="HL4" s="71"/>
-      <c r="HM4" s="71"/>
-      <c r="HN4" s="71"/>
-      <c r="HO4" s="71"/>
-      <c r="HP4" s="71"/>
-      <c r="HQ4" s="71"/>
-      <c r="HR4" s="71"/>
-      <c r="HS4" s="71"/>
-      <c r="HT4" s="71"/>
-      <c r="HU4" s="71"/>
-      <c r="HV4" s="71"/>
-      <c r="HW4" s="88" t="s">
+      <c r="HJ4" s="67"/>
+      <c r="HK4" s="67"/>
+      <c r="HL4" s="67"/>
+      <c r="HM4" s="67"/>
+      <c r="HN4" s="67"/>
+      <c r="HO4" s="67"/>
+      <c r="HP4" s="67"/>
+      <c r="HQ4" s="67"/>
+      <c r="HR4" s="67"/>
+      <c r="HS4" s="67"/>
+      <c r="HT4" s="67"/>
+      <c r="HU4" s="67"/>
+      <c r="HV4" s="67"/>
+      <c r="HW4" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="88"/>
-      <c r="HY4" s="88"/>
-      <c r="HZ4" s="88"/>
-      <c r="IA4" s="88"/>
-      <c r="IB4" s="88"/>
-      <c r="IC4" s="88"/>
-      <c r="ID4" s="88"/>
-      <c r="IE4" s="88"/>
-      <c r="IF4" s="88"/>
-      <c r="IG4" s="88"/>
-      <c r="IH4" s="88"/>
-      <c r="II4" s="88"/>
-      <c r="IJ4" s="88"/>
-      <c r="IK4" s="88" t="s">
+      <c r="HX4" s="68"/>
+      <c r="HY4" s="68"/>
+      <c r="HZ4" s="68"/>
+      <c r="IA4" s="68"/>
+      <c r="IB4" s="68"/>
+      <c r="IC4" s="68"/>
+      <c r="ID4" s="68"/>
+      <c r="IE4" s="68"/>
+      <c r="IF4" s="68"/>
+      <c r="IG4" s="68"/>
+      <c r="IH4" s="68"/>
+      <c r="II4" s="68"/>
+      <c r="IJ4" s="68"/>
+      <c r="IK4" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="88"/>
-      <c r="IM4" s="88"/>
-      <c r="IN4" s="88"/>
-      <c r="IO4" s="88"/>
-      <c r="IP4" s="88"/>
-      <c r="IQ4" s="88"/>
-      <c r="IR4" s="88"/>
-      <c r="IS4" s="88"/>
-      <c r="IT4" s="88"/>
-      <c r="IU4" s="88"/>
-      <c r="IV4" s="88"/>
-      <c r="IW4" s="88"/>
-      <c r="IX4" s="88"/>
-      <c r="IY4" s="88" t="s">
+      <c r="IL4" s="68"/>
+      <c r="IM4" s="68"/>
+      <c r="IN4" s="68"/>
+      <c r="IO4" s="68"/>
+      <c r="IP4" s="68"/>
+      <c r="IQ4" s="68"/>
+      <c r="IR4" s="68"/>
+      <c r="IS4" s="68"/>
+      <c r="IT4" s="68"/>
+      <c r="IU4" s="68"/>
+      <c r="IV4" s="68"/>
+      <c r="IW4" s="68"/>
+      <c r="IX4" s="68"/>
+      <c r="IY4" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="88"/>
-      <c r="JA4" s="88"/>
-      <c r="JB4" s="88"/>
-      <c r="JC4" s="88"/>
-      <c r="JD4" s="88"/>
-      <c r="JE4" s="88"/>
-      <c r="JF4" s="88"/>
-      <c r="JG4" s="88"/>
-      <c r="JH4" s="88"/>
-      <c r="JI4" s="88"/>
-      <c r="JJ4" s="88"/>
-      <c r="JK4" s="88"/>
-      <c r="JL4" s="88"/>
-      <c r="JM4" s="89" t="s">
+      <c r="IZ4" s="68"/>
+      <c r="JA4" s="68"/>
+      <c r="JB4" s="68"/>
+      <c r="JC4" s="68"/>
+      <c r="JD4" s="68"/>
+      <c r="JE4" s="68"/>
+      <c r="JF4" s="68"/>
+      <c r="JG4" s="68"/>
+      <c r="JH4" s="68"/>
+      <c r="JI4" s="68"/>
+      <c r="JJ4" s="68"/>
+      <c r="JK4" s="68"/>
+      <c r="JL4" s="68"/>
+      <c r="JM4" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="89"/>
-      <c r="JO4" s="89"/>
-      <c r="JP4" s="89"/>
-      <c r="JQ4" s="89"/>
-      <c r="JR4" s="89"/>
-      <c r="JS4" s="89"/>
-      <c r="JT4" s="89"/>
-      <c r="JU4" s="89"/>
-      <c r="JV4" s="89"/>
-      <c r="JW4" s="89"/>
-      <c r="JX4" s="89"/>
-      <c r="JY4" s="89"/>
-      <c r="JZ4" s="86" t="s">
+      <c r="JN4" s="69"/>
+      <c r="JO4" s="69"/>
+      <c r="JP4" s="69"/>
+      <c r="JQ4" s="69"/>
+      <c r="JR4" s="69"/>
+      <c r="JS4" s="69"/>
+      <c r="JT4" s="69"/>
+      <c r="JU4" s="69"/>
+      <c r="JV4" s="69"/>
+      <c r="JW4" s="69"/>
+      <c r="JX4" s="69"/>
+      <c r="JY4" s="69"/>
+      <c r="JZ4" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="87"/>
-      <c r="KB4" s="87"/>
-      <c r="KC4" s="87"/>
-      <c r="KD4" s="87"/>
-      <c r="KE4" s="87"/>
-      <c r="KF4" s="87"/>
-      <c r="KG4" s="87"/>
-      <c r="KH4" s="82" t="s">
+      <c r="KA4" s="66"/>
+      <c r="KB4" s="66"/>
+      <c r="KC4" s="66"/>
+      <c r="KD4" s="66"/>
+      <c r="KE4" s="66"/>
+      <c r="KF4" s="66"/>
+      <c r="KG4" s="66"/>
+      <c r="KH4" s="61" t="s">
         <v>322</v>
       </c>
-      <c r="KI4" s="83"/>
-      <c r="KJ4" s="83"/>
-      <c r="KK4" s="83"/>
+      <c r="KI4" s="62"/>
+      <c r="KJ4" s="62"/>
+      <c r="KK4" s="62"/>
       <c r="KL4" s="60"/>
     </row>
-    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="68"/>
-      <c r="V5" s="68"/>
-      <c r="W5" s="68"/>
-      <c r="X5" s="68"/>
-      <c r="Y5" s="68"/>
-      <c r="Z5" s="68"/>
-      <c r="AA5" s="68"/>
-      <c r="AB5" s="68"/>
-      <c r="AC5" s="69"/>
-      <c r="AD5" s="69"/>
-      <c r="AE5" s="69"/>
-      <c r="AF5" s="69"/>
-      <c r="AG5" s="69"/>
-      <c r="AH5" s="69"/>
-      <c r="AI5" s="69"/>
-      <c r="AJ5" s="70"/>
-      <c r="AK5" s="70"/>
-      <c r="AL5" s="70"/>
-      <c r="AM5" s="61"/>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="72"/>
-      <c r="AP5" s="72"/>
-      <c r="AQ5" s="72"/>
-      <c r="AR5" s="72"/>
-      <c r="AS5" s="73"/>
-      <c r="AT5" s="73"/>
-      <c r="AU5" s="73"/>
-      <c r="AV5" s="73"/>
-      <c r="AW5" s="73"/>
-      <c r="AX5" s="73"/>
-      <c r="AY5" s="73"/>
-      <c r="AZ5" s="73"/>
-      <c r="BA5" s="73"/>
-      <c r="BB5" s="73"/>
-      <c r="BC5" s="73"/>
-      <c r="BD5" s="73"/>
-      <c r="BE5" s="73"/>
-      <c r="BF5" s="73"/>
-      <c r="BG5" s="73"/>
-      <c r="BH5" s="73"/>
-      <c r="BI5" s="73"/>
-      <c r="BJ5" s="73"/>
+    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="83"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
+      <c r="AB5" s="87"/>
+      <c r="AC5" s="88"/>
+      <c r="AD5" s="88"/>
+      <c r="AE5" s="88"/>
+      <c r="AF5" s="88"/>
+      <c r="AG5" s="88"/>
+      <c r="AH5" s="88"/>
+      <c r="AI5" s="88"/>
+      <c r="AJ5" s="89"/>
+      <c r="AK5" s="89"/>
+      <c r="AL5" s="89"/>
+      <c r="AM5" s="80"/>
+      <c r="AN5" s="80"/>
+      <c r="AO5" s="70"/>
+      <c r="AP5" s="70"/>
+      <c r="AQ5" s="70"/>
+      <c r="AR5" s="70"/>
+      <c r="AS5" s="71"/>
+      <c r="AT5" s="71"/>
+      <c r="AU5" s="71"/>
+      <c r="AV5" s="71"/>
+      <c r="AW5" s="71"/>
+      <c r="AX5" s="71"/>
+      <c r="AY5" s="71"/>
+      <c r="AZ5" s="71"/>
+      <c r="BA5" s="71"/>
+      <c r="BB5" s="71"/>
+      <c r="BC5" s="71"/>
+      <c r="BD5" s="71"/>
+      <c r="BE5" s="71"/>
+      <c r="BF5" s="71"/>
+      <c r="BG5" s="71"/>
+      <c r="BH5" s="71"/>
+      <c r="BI5" s="71"/>
+      <c r="BJ5" s="71"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4463,38 +4471,38 @@
       <c r="JL5" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="JM5" s="89"/>
-      <c r="JN5" s="89"/>
-      <c r="JO5" s="89"/>
-      <c r="JP5" s="89"/>
-      <c r="JQ5" s="89"/>
-      <c r="JR5" s="89"/>
-      <c r="JS5" s="89"/>
-      <c r="JT5" s="89"/>
-      <c r="JU5" s="89"/>
-      <c r="JV5" s="89"/>
-      <c r="JW5" s="89"/>
-      <c r="JX5" s="89"/>
-      <c r="JY5" s="89"/>
-      <c r="JZ5" s="87" t="s">
+      <c r="JM5" s="69"/>
+      <c r="JN5" s="69"/>
+      <c r="JO5" s="69"/>
+      <c r="JP5" s="69"/>
+      <c r="JQ5" s="69"/>
+      <c r="JR5" s="69"/>
+      <c r="JS5" s="69"/>
+      <c r="JT5" s="69"/>
+      <c r="JU5" s="69"/>
+      <c r="JV5" s="69"/>
+      <c r="JW5" s="69"/>
+      <c r="JX5" s="69"/>
+      <c r="JY5" s="69"/>
+      <c r="JZ5" s="66" t="s">
         <v>316</v>
       </c>
-      <c r="KA5" s="87"/>
-      <c r="KB5" s="87"/>
-      <c r="KC5" s="87"/>
-      <c r="KD5" s="87" t="s">
+      <c r="KA5" s="66"/>
+      <c r="KB5" s="66"/>
+      <c r="KC5" s="66"/>
+      <c r="KD5" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="87"/>
-      <c r="KF5" s="87"/>
-      <c r="KG5" s="87"/>
-      <c r="KH5" s="84"/>
-      <c r="KI5" s="85"/>
-      <c r="KJ5" s="85"/>
-      <c r="KK5" s="85"/>
+      <c r="KE5" s="66"/>
+      <c r="KF5" s="66"/>
+      <c r="KG5" s="66"/>
+      <c r="KH5" s="63"/>
+      <c r="KI5" s="64"/>
+      <c r="KJ5" s="64"/>
+      <c r="KK5" s="64"/>
       <c r="KL5" s="60"/>
     </row>
-    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -5390,7 +5398,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>343</v>
       </c>
@@ -6312,7 +6320,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="8" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>365</v>
       </c>
@@ -7234,7 +7242,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="9" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>378</v>
       </c>
@@ -8156,7 +8164,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="10" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>397</v>
       </c>
@@ -9078,7 +9086,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="11" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>408</v>
       </c>
@@ -10001,22 +10009,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KK6">
-    <sortState ref="A7:KK10">
+  <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:KK10">
       <sortCondition ref="KK6"/>
     </sortState>
   </autoFilter>
   <mergeCells count="32">
-    <mergeCell ref="KH4:KK5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -10029,31 +10037,31 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KK5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="4">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR11">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7:KI11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7:KI11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7:KK11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7:KK11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"NGSA, WEM, FCRM Operational Framework, Other, Unknown/TBC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7:KH11 KJ7:KJ11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7:KH11 KJ7:KJ11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10061,4 +10069,16 @@
   <pageSetup paperSize="9" scale="10" orientation="landscape"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BBB8C6-3FA0-4446-A91C-24D37E1D0F94}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[PM-498] Update expected probgram spreadsheet to include FC page
</commit_message>
<xml_diff>
--- a/spec/fixtures/expected_program_spreadsheet.xlsx
+++ b/spec/fixtures/expected_program_spreadsheet.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selks\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthall/Work/pafs/pafs_core/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB64377-04B4-3843-B331-791D09F1FE48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="11388"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15760" windowHeight="11380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master local choices" sheetId="2" r:id="rId1"/>
+    <sheet name="Funding Contributors" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master local choices'!$A$6:$KK$6</definedName>
@@ -90,22 +92,28 @@
     <definedName name="wages_freq_int_rec" localSheetId="0">#REF!</definedName>
     <definedName name="wages_freq_int_rec">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Registered User</author>
   </authors>
   <commentList>
-    <comment ref="CD6" authorId="0" shapeId="0">
+    <comment ref="CD6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1485,13 +1493,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
-    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    <numFmt numFmtId="167" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="168" formatCode="#,##0.0_ ;[Red]\-#,##0.0\ "/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1817,7 +1825,7 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -1891,7 +1899,7 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1911,22 +1919,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1935,10 +1943,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1992,7 +2000,7 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2000,37 +2008,31 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="11" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2063,41 +2065,47 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="%" xfId="3"/>
-    <cellStyle name="% 2 2 2" xfId="4"/>
+    <cellStyle name="%" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% 2 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="8"/>
-    <cellStyle name="Normal 2 2" xfId="6"/>
-    <cellStyle name="Normal_RCP" xfId="5"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
-    <cellStyle name="Percent 11" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal_RCP" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent 11" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2486,14 +2494,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:KL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
@@ -2501,9 +2509,9 @@
       <selection pane="bottomRight" activeCell="KL18" sqref="KL18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54" style="1" customWidth="1"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="6" width="21" style="1" customWidth="1"/>
@@ -2521,17 +2529,17 @@
     <col min="45" max="278" width="21" style="1" customWidth="1"/>
     <col min="279" max="285" width="21" style="29" customWidth="1"/>
     <col min="286" max="293" width="21" style="6" customWidth="1"/>
-    <col min="294" max="296" width="22.1796875" style="7" customWidth="1"/>
-    <col min="297" max="297" width="13.1796875" style="7" customWidth="1"/>
+    <col min="294" max="296" width="22.140625" style="7" customWidth="1"/>
+    <col min="297" max="297" width="13.140625" style="7" customWidth="1"/>
     <col min="298" max="298" width="11" style="7" customWidth="1"/>
-    <col min="299" max="16384" width="8.81640625" style="7"/>
+    <col min="299" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="62"/>
+    <row r="1" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81"/>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
       <c r="E1" s="23"/>
@@ -2824,11 +2832,11 @@
       <c r="KF1" s="23"/>
       <c r="KG1" s="23"/>
     </row>
-    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+    <row r="2" spans="1:298" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="82" t="s">
         <v>320</v>
       </c>
-      <c r="B2" s="63"/>
+      <c r="B2" s="82"/>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
       <c r="E2" s="23"/>
@@ -3121,7 +3129,7 @@
       <c r="KF2" s="42"/>
       <c r="KG2" s="42"/>
     </row>
-    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:298" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="44"/>
@@ -3416,423 +3424,423 @@
       <c r="KF3" s="50"/>
       <c r="KG3" s="50"/>
     </row>
-    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+    <row r="4" spans="1:298" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65" t="s">
+      <c r="B4" s="83"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="66" t="s">
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="67" t="s">
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
-      <c r="U4" s="68" t="s">
+      <c r="Q4" s="86"/>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="68"/>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="68"/>
-      <c r="Z4" s="68"/>
-      <c r="AA4" s="68"/>
-      <c r="AB4" s="68"/>
-      <c r="AC4" s="69" t="s">
+      <c r="V4" s="87"/>
+      <c r="W4" s="87"/>
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="AD4" s="69"/>
-      <c r="AE4" s="69"/>
-      <c r="AF4" s="69"/>
-      <c r="AG4" s="69"/>
-      <c r="AH4" s="69"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="70" t="s">
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="88"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="AK4" s="70"/>
-      <c r="AL4" s="70"/>
-      <c r="AM4" s="61" t="s">
+      <c r="AK4" s="89"/>
+      <c r="AL4" s="89"/>
+      <c r="AM4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="72"/>
-      <c r="AP4" s="72"/>
-      <c r="AQ4" s="72"/>
-      <c r="AR4" s="72"/>
-      <c r="AS4" s="73" t="s">
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="70"/>
+      <c r="AQ4" s="70"/>
+      <c r="AR4" s="70"/>
+      <c r="AS4" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="AT4" s="73"/>
-      <c r="AU4" s="73"/>
-      <c r="AV4" s="73"/>
-      <c r="AW4" s="73"/>
-      <c r="AX4" s="73"/>
-      <c r="AY4" s="73"/>
-      <c r="AZ4" s="73"/>
-      <c r="BA4" s="73"/>
-      <c r="BB4" s="73"/>
-      <c r="BC4" s="73"/>
-      <c r="BD4" s="73"/>
-      <c r="BE4" s="73"/>
-      <c r="BF4" s="73"/>
-      <c r="BG4" s="73"/>
-      <c r="BH4" s="73"/>
-      <c r="BI4" s="73"/>
-      <c r="BJ4" s="73"/>
-      <c r="BK4" s="71" t="s">
+      <c r="AT4" s="71"/>
+      <c r="AU4" s="71"/>
+      <c r="AV4" s="71"/>
+      <c r="AW4" s="71"/>
+      <c r="AX4" s="71"/>
+      <c r="AY4" s="71"/>
+      <c r="AZ4" s="71"/>
+      <c r="BA4" s="71"/>
+      <c r="BB4" s="71"/>
+      <c r="BC4" s="71"/>
+      <c r="BD4" s="71"/>
+      <c r="BE4" s="71"/>
+      <c r="BF4" s="71"/>
+      <c r="BG4" s="71"/>
+      <c r="BH4" s="71"/>
+      <c r="BI4" s="71"/>
+      <c r="BJ4" s="71"/>
+      <c r="BK4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="BL4" s="71"/>
-      <c r="BM4" s="71"/>
-      <c r="BN4" s="71"/>
-      <c r="BO4" s="71"/>
-      <c r="BP4" s="71"/>
-      <c r="BQ4" s="71"/>
-      <c r="BR4" s="71"/>
-      <c r="BS4" s="71"/>
-      <c r="BT4" s="71"/>
-      <c r="BU4" s="71"/>
-      <c r="BV4" s="71"/>
-      <c r="BW4" s="71"/>
-      <c r="BX4" s="71"/>
-      <c r="BY4" s="74" t="s">
+      <c r="BL4" s="67"/>
+      <c r="BM4" s="67"/>
+      <c r="BN4" s="67"/>
+      <c r="BO4" s="67"/>
+      <c r="BP4" s="67"/>
+      <c r="BQ4" s="67"/>
+      <c r="BR4" s="67"/>
+      <c r="BS4" s="67"/>
+      <c r="BT4" s="67"/>
+      <c r="BU4" s="67"/>
+      <c r="BV4" s="67"/>
+      <c r="BW4" s="67"/>
+      <c r="BX4" s="67"/>
+      <c r="BY4" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="BZ4" s="74"/>
-      <c r="CA4" s="74"/>
-      <c r="CB4" s="74"/>
-      <c r="CC4" s="74"/>
-      <c r="CD4" s="74"/>
-      <c r="CE4" s="74"/>
-      <c r="CF4" s="74"/>
-      <c r="CG4" s="74"/>
-      <c r="CH4" s="74"/>
-      <c r="CI4" s="74"/>
-      <c r="CJ4" s="74"/>
-      <c r="CK4" s="74"/>
-      <c r="CL4" s="74"/>
-      <c r="CM4" s="75" t="s">
+      <c r="BZ4" s="72"/>
+      <c r="CA4" s="72"/>
+      <c r="CB4" s="72"/>
+      <c r="CC4" s="72"/>
+      <c r="CD4" s="72"/>
+      <c r="CE4" s="72"/>
+      <c r="CF4" s="72"/>
+      <c r="CG4" s="72"/>
+      <c r="CH4" s="72"/>
+      <c r="CI4" s="72"/>
+      <c r="CJ4" s="72"/>
+      <c r="CK4" s="72"/>
+      <c r="CL4" s="72"/>
+      <c r="CM4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="CN4" s="75"/>
-      <c r="CO4" s="75"/>
-      <c r="CP4" s="75"/>
-      <c r="CQ4" s="75"/>
-      <c r="CR4" s="75"/>
-      <c r="CS4" s="75"/>
-      <c r="CT4" s="75"/>
-      <c r="CU4" s="75"/>
-      <c r="CV4" s="75"/>
-      <c r="CW4" s="75"/>
-      <c r="CX4" s="75"/>
-      <c r="CY4" s="75"/>
-      <c r="CZ4" s="75"/>
-      <c r="DA4" s="76" t="s">
+      <c r="CN4" s="73"/>
+      <c r="CO4" s="73"/>
+      <c r="CP4" s="73"/>
+      <c r="CQ4" s="73"/>
+      <c r="CR4" s="73"/>
+      <c r="CS4" s="73"/>
+      <c r="CT4" s="73"/>
+      <c r="CU4" s="73"/>
+      <c r="CV4" s="73"/>
+      <c r="CW4" s="73"/>
+      <c r="CX4" s="73"/>
+      <c r="CY4" s="73"/>
+      <c r="CZ4" s="73"/>
+      <c r="DA4" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="DB4" s="76"/>
-      <c r="DC4" s="76"/>
-      <c r="DD4" s="76"/>
-      <c r="DE4" s="76"/>
-      <c r="DF4" s="76"/>
-      <c r="DG4" s="76"/>
-      <c r="DH4" s="76"/>
-      <c r="DI4" s="76"/>
-      <c r="DJ4" s="76"/>
-      <c r="DK4" s="76"/>
-      <c r="DL4" s="76"/>
-      <c r="DM4" s="76"/>
-      <c r="DN4" s="76"/>
-      <c r="DO4" s="77" t="s">
+      <c r="DB4" s="74"/>
+      <c r="DC4" s="74"/>
+      <c r="DD4" s="74"/>
+      <c r="DE4" s="74"/>
+      <c r="DF4" s="74"/>
+      <c r="DG4" s="74"/>
+      <c r="DH4" s="74"/>
+      <c r="DI4" s="74"/>
+      <c r="DJ4" s="74"/>
+      <c r="DK4" s="74"/>
+      <c r="DL4" s="74"/>
+      <c r="DM4" s="74"/>
+      <c r="DN4" s="74"/>
+      <c r="DO4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="DP4" s="77"/>
-      <c r="DQ4" s="77"/>
-      <c r="DR4" s="77"/>
-      <c r="DS4" s="77"/>
-      <c r="DT4" s="77"/>
-      <c r="DU4" s="77"/>
-      <c r="DV4" s="77"/>
-      <c r="DW4" s="77"/>
-      <c r="DX4" s="77"/>
-      <c r="DY4" s="77"/>
-      <c r="DZ4" s="77"/>
-      <c r="EA4" s="77"/>
-      <c r="EB4" s="77"/>
-      <c r="EC4" s="78" t="s">
+      <c r="DP4" s="75"/>
+      <c r="DQ4" s="75"/>
+      <c r="DR4" s="75"/>
+      <c r="DS4" s="75"/>
+      <c r="DT4" s="75"/>
+      <c r="DU4" s="75"/>
+      <c r="DV4" s="75"/>
+      <c r="DW4" s="75"/>
+      <c r="DX4" s="75"/>
+      <c r="DY4" s="75"/>
+      <c r="DZ4" s="75"/>
+      <c r="EA4" s="75"/>
+      <c r="EB4" s="75"/>
+      <c r="EC4" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="ED4" s="78"/>
-      <c r="EE4" s="78"/>
-      <c r="EF4" s="78"/>
-      <c r="EG4" s="78"/>
-      <c r="EH4" s="78"/>
-      <c r="EI4" s="78"/>
-      <c r="EJ4" s="78"/>
-      <c r="EK4" s="78"/>
-      <c r="EL4" s="78"/>
-      <c r="EM4" s="78"/>
-      <c r="EN4" s="78"/>
-      <c r="EO4" s="78"/>
-      <c r="EP4" s="78"/>
-      <c r="EQ4" s="79" t="s">
+      <c r="ED4" s="76"/>
+      <c r="EE4" s="76"/>
+      <c r="EF4" s="76"/>
+      <c r="EG4" s="76"/>
+      <c r="EH4" s="76"/>
+      <c r="EI4" s="76"/>
+      <c r="EJ4" s="76"/>
+      <c r="EK4" s="76"/>
+      <c r="EL4" s="76"/>
+      <c r="EM4" s="76"/>
+      <c r="EN4" s="76"/>
+      <c r="EO4" s="76"/>
+      <c r="EP4" s="76"/>
+      <c r="EQ4" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="ER4" s="79"/>
-      <c r="ES4" s="79"/>
-      <c r="ET4" s="79"/>
-      <c r="EU4" s="79"/>
-      <c r="EV4" s="79"/>
-      <c r="EW4" s="79"/>
-      <c r="EX4" s="79"/>
-      <c r="EY4" s="79"/>
-      <c r="EZ4" s="79"/>
-      <c r="FA4" s="79"/>
-      <c r="FB4" s="79"/>
-      <c r="FC4" s="79"/>
-      <c r="FD4" s="79"/>
-      <c r="FE4" s="80" t="s">
+      <c r="ER4" s="77"/>
+      <c r="ES4" s="77"/>
+      <c r="ET4" s="77"/>
+      <c r="EU4" s="77"/>
+      <c r="EV4" s="77"/>
+      <c r="EW4" s="77"/>
+      <c r="EX4" s="77"/>
+      <c r="EY4" s="77"/>
+      <c r="EZ4" s="77"/>
+      <c r="FA4" s="77"/>
+      <c r="FB4" s="77"/>
+      <c r="FC4" s="77"/>
+      <c r="FD4" s="77"/>
+      <c r="FE4" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="FF4" s="80"/>
-      <c r="FG4" s="80"/>
-      <c r="FH4" s="80"/>
-      <c r="FI4" s="80"/>
-      <c r="FJ4" s="80"/>
-      <c r="FK4" s="80"/>
-      <c r="FL4" s="80"/>
-      <c r="FM4" s="80"/>
-      <c r="FN4" s="80"/>
-      <c r="FO4" s="80"/>
-      <c r="FP4" s="80"/>
-      <c r="FQ4" s="80"/>
-      <c r="FR4" s="80"/>
-      <c r="FS4" s="81" t="s">
+      <c r="FF4" s="78"/>
+      <c r="FG4" s="78"/>
+      <c r="FH4" s="78"/>
+      <c r="FI4" s="78"/>
+      <c r="FJ4" s="78"/>
+      <c r="FK4" s="78"/>
+      <c r="FL4" s="78"/>
+      <c r="FM4" s="78"/>
+      <c r="FN4" s="78"/>
+      <c r="FO4" s="78"/>
+      <c r="FP4" s="78"/>
+      <c r="FQ4" s="78"/>
+      <c r="FR4" s="78"/>
+      <c r="FS4" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="FT4" s="81"/>
-      <c r="FU4" s="81"/>
-      <c r="FV4" s="81"/>
-      <c r="FW4" s="81"/>
-      <c r="FX4" s="81"/>
-      <c r="FY4" s="81"/>
-      <c r="FZ4" s="81"/>
-      <c r="GA4" s="81"/>
-      <c r="GB4" s="81"/>
-      <c r="GC4" s="81"/>
-      <c r="GD4" s="81"/>
-      <c r="GE4" s="81"/>
-      <c r="GF4" s="81"/>
-      <c r="GG4" s="71" t="s">
+      <c r="FT4" s="79"/>
+      <c r="FU4" s="79"/>
+      <c r="FV4" s="79"/>
+      <c r="FW4" s="79"/>
+      <c r="FX4" s="79"/>
+      <c r="FY4" s="79"/>
+      <c r="FZ4" s="79"/>
+      <c r="GA4" s="79"/>
+      <c r="GB4" s="79"/>
+      <c r="GC4" s="79"/>
+      <c r="GD4" s="79"/>
+      <c r="GE4" s="79"/>
+      <c r="GF4" s="79"/>
+      <c r="GG4" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="GH4" s="71"/>
-      <c r="GI4" s="71"/>
-      <c r="GJ4" s="71"/>
-      <c r="GK4" s="71"/>
-      <c r="GL4" s="71"/>
-      <c r="GM4" s="71"/>
-      <c r="GN4" s="71"/>
-      <c r="GO4" s="71"/>
-      <c r="GP4" s="71"/>
-      <c r="GQ4" s="71"/>
-      <c r="GR4" s="71"/>
-      <c r="GS4" s="71"/>
-      <c r="GT4" s="71"/>
-      <c r="GU4" s="71" t="s">
+      <c r="GH4" s="67"/>
+      <c r="GI4" s="67"/>
+      <c r="GJ4" s="67"/>
+      <c r="GK4" s="67"/>
+      <c r="GL4" s="67"/>
+      <c r="GM4" s="67"/>
+      <c r="GN4" s="67"/>
+      <c r="GO4" s="67"/>
+      <c r="GP4" s="67"/>
+      <c r="GQ4" s="67"/>
+      <c r="GR4" s="67"/>
+      <c r="GS4" s="67"/>
+      <c r="GT4" s="67"/>
+      <c r="GU4" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="GV4" s="71"/>
-      <c r="GW4" s="71"/>
-      <c r="GX4" s="71"/>
-      <c r="GY4" s="71"/>
-      <c r="GZ4" s="71"/>
-      <c r="HA4" s="71"/>
-      <c r="HB4" s="71"/>
-      <c r="HC4" s="71"/>
-      <c r="HD4" s="71"/>
-      <c r="HE4" s="71"/>
-      <c r="HF4" s="71"/>
-      <c r="HG4" s="71"/>
-      <c r="HH4" s="71"/>
-      <c r="HI4" s="71" t="s">
+      <c r="GV4" s="67"/>
+      <c r="GW4" s="67"/>
+      <c r="GX4" s="67"/>
+      <c r="GY4" s="67"/>
+      <c r="GZ4" s="67"/>
+      <c r="HA4" s="67"/>
+      <c r="HB4" s="67"/>
+      <c r="HC4" s="67"/>
+      <c r="HD4" s="67"/>
+      <c r="HE4" s="67"/>
+      <c r="HF4" s="67"/>
+      <c r="HG4" s="67"/>
+      <c r="HH4" s="67"/>
+      <c r="HI4" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="HJ4" s="71"/>
-      <c r="HK4" s="71"/>
-      <c r="HL4" s="71"/>
-      <c r="HM4" s="71"/>
-      <c r="HN4" s="71"/>
-      <c r="HO4" s="71"/>
-      <c r="HP4" s="71"/>
-      <c r="HQ4" s="71"/>
-      <c r="HR4" s="71"/>
-      <c r="HS4" s="71"/>
-      <c r="HT4" s="71"/>
-      <c r="HU4" s="71"/>
-      <c r="HV4" s="71"/>
-      <c r="HW4" s="88" t="s">
+      <c r="HJ4" s="67"/>
+      <c r="HK4" s="67"/>
+      <c r="HL4" s="67"/>
+      <c r="HM4" s="67"/>
+      <c r="HN4" s="67"/>
+      <c r="HO4" s="67"/>
+      <c r="HP4" s="67"/>
+      <c r="HQ4" s="67"/>
+      <c r="HR4" s="67"/>
+      <c r="HS4" s="67"/>
+      <c r="HT4" s="67"/>
+      <c r="HU4" s="67"/>
+      <c r="HV4" s="67"/>
+      <c r="HW4" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="HX4" s="88"/>
-      <c r="HY4" s="88"/>
-      <c r="HZ4" s="88"/>
-      <c r="IA4" s="88"/>
-      <c r="IB4" s="88"/>
-      <c r="IC4" s="88"/>
-      <c r="ID4" s="88"/>
-      <c r="IE4" s="88"/>
-      <c r="IF4" s="88"/>
-      <c r="IG4" s="88"/>
-      <c r="IH4" s="88"/>
-      <c r="II4" s="88"/>
-      <c r="IJ4" s="88"/>
-      <c r="IK4" s="88" t="s">
+      <c r="HX4" s="68"/>
+      <c r="HY4" s="68"/>
+      <c r="HZ4" s="68"/>
+      <c r="IA4" s="68"/>
+      <c r="IB4" s="68"/>
+      <c r="IC4" s="68"/>
+      <c r="ID4" s="68"/>
+      <c r="IE4" s="68"/>
+      <c r="IF4" s="68"/>
+      <c r="IG4" s="68"/>
+      <c r="IH4" s="68"/>
+      <c r="II4" s="68"/>
+      <c r="IJ4" s="68"/>
+      <c r="IK4" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="IL4" s="88"/>
-      <c r="IM4" s="88"/>
-      <c r="IN4" s="88"/>
-      <c r="IO4" s="88"/>
-      <c r="IP4" s="88"/>
-      <c r="IQ4" s="88"/>
-      <c r="IR4" s="88"/>
-      <c r="IS4" s="88"/>
-      <c r="IT4" s="88"/>
-      <c r="IU4" s="88"/>
-      <c r="IV4" s="88"/>
-      <c r="IW4" s="88"/>
-      <c r="IX4" s="88"/>
-      <c r="IY4" s="88" t="s">
+      <c r="IL4" s="68"/>
+      <c r="IM4" s="68"/>
+      <c r="IN4" s="68"/>
+      <c r="IO4" s="68"/>
+      <c r="IP4" s="68"/>
+      <c r="IQ4" s="68"/>
+      <c r="IR4" s="68"/>
+      <c r="IS4" s="68"/>
+      <c r="IT4" s="68"/>
+      <c r="IU4" s="68"/>
+      <c r="IV4" s="68"/>
+      <c r="IW4" s="68"/>
+      <c r="IX4" s="68"/>
+      <c r="IY4" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="IZ4" s="88"/>
-      <c r="JA4" s="88"/>
-      <c r="JB4" s="88"/>
-      <c r="JC4" s="88"/>
-      <c r="JD4" s="88"/>
-      <c r="JE4" s="88"/>
-      <c r="JF4" s="88"/>
-      <c r="JG4" s="88"/>
-      <c r="JH4" s="88"/>
-      <c r="JI4" s="88"/>
-      <c r="JJ4" s="88"/>
-      <c r="JK4" s="88"/>
-      <c r="JL4" s="88"/>
-      <c r="JM4" s="89" t="s">
+      <c r="IZ4" s="68"/>
+      <c r="JA4" s="68"/>
+      <c r="JB4" s="68"/>
+      <c r="JC4" s="68"/>
+      <c r="JD4" s="68"/>
+      <c r="JE4" s="68"/>
+      <c r="JF4" s="68"/>
+      <c r="JG4" s="68"/>
+      <c r="JH4" s="68"/>
+      <c r="JI4" s="68"/>
+      <c r="JJ4" s="68"/>
+      <c r="JK4" s="68"/>
+      <c r="JL4" s="68"/>
+      <c r="JM4" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="JN4" s="89"/>
-      <c r="JO4" s="89"/>
-      <c r="JP4" s="89"/>
-      <c r="JQ4" s="89"/>
-      <c r="JR4" s="89"/>
-      <c r="JS4" s="89"/>
-      <c r="JT4" s="89"/>
-      <c r="JU4" s="89"/>
-      <c r="JV4" s="89"/>
-      <c r="JW4" s="89"/>
-      <c r="JX4" s="89"/>
-      <c r="JY4" s="89"/>
-      <c r="JZ4" s="86" t="s">
+      <c r="JN4" s="69"/>
+      <c r="JO4" s="69"/>
+      <c r="JP4" s="69"/>
+      <c r="JQ4" s="69"/>
+      <c r="JR4" s="69"/>
+      <c r="JS4" s="69"/>
+      <c r="JT4" s="69"/>
+      <c r="JU4" s="69"/>
+      <c r="JV4" s="69"/>
+      <c r="JW4" s="69"/>
+      <c r="JX4" s="69"/>
+      <c r="JY4" s="69"/>
+      <c r="JZ4" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="KA4" s="87"/>
-      <c r="KB4" s="87"/>
-      <c r="KC4" s="87"/>
-      <c r="KD4" s="87"/>
-      <c r="KE4" s="87"/>
-      <c r="KF4" s="87"/>
-      <c r="KG4" s="87"/>
-      <c r="KH4" s="82" t="s">
+      <c r="KA4" s="66"/>
+      <c r="KB4" s="66"/>
+      <c r="KC4" s="66"/>
+      <c r="KD4" s="66"/>
+      <c r="KE4" s="66"/>
+      <c r="KF4" s="66"/>
+      <c r="KG4" s="66"/>
+      <c r="KH4" s="61" t="s">
         <v>322</v>
       </c>
-      <c r="KI4" s="83"/>
-      <c r="KJ4" s="83"/>
-      <c r="KK4" s="83"/>
+      <c r="KI4" s="62"/>
+      <c r="KJ4" s="62"/>
+      <c r="KK4" s="62"/>
       <c r="KL4" s="60"/>
     </row>
-    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="67"/>
-      <c r="U5" s="68"/>
-      <c r="V5" s="68"/>
-      <c r="W5" s="68"/>
-      <c r="X5" s="68"/>
-      <c r="Y5" s="68"/>
-      <c r="Z5" s="68"/>
-      <c r="AA5" s="68"/>
-      <c r="AB5" s="68"/>
-      <c r="AC5" s="69"/>
-      <c r="AD5" s="69"/>
-      <c r="AE5" s="69"/>
-      <c r="AF5" s="69"/>
-      <c r="AG5" s="69"/>
-      <c r="AH5" s="69"/>
-      <c r="AI5" s="69"/>
-      <c r="AJ5" s="70"/>
-      <c r="AK5" s="70"/>
-      <c r="AL5" s="70"/>
-      <c r="AM5" s="61"/>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="72"/>
-      <c r="AP5" s="72"/>
-      <c r="AQ5" s="72"/>
-      <c r="AR5" s="72"/>
-      <c r="AS5" s="73"/>
-      <c r="AT5" s="73"/>
-      <c r="AU5" s="73"/>
-      <c r="AV5" s="73"/>
-      <c r="AW5" s="73"/>
-      <c r="AX5" s="73"/>
-      <c r="AY5" s="73"/>
-      <c r="AZ5" s="73"/>
-      <c r="BA5" s="73"/>
-      <c r="BB5" s="73"/>
-      <c r="BC5" s="73"/>
-      <c r="BD5" s="73"/>
-      <c r="BE5" s="73"/>
-      <c r="BF5" s="73"/>
-      <c r="BG5" s="73"/>
-      <c r="BH5" s="73"/>
-      <c r="BI5" s="73"/>
-      <c r="BJ5" s="73"/>
+    <row r="5" spans="1:298" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="83"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
+      <c r="AB5" s="87"/>
+      <c r="AC5" s="88"/>
+      <c r="AD5" s="88"/>
+      <c r="AE5" s="88"/>
+      <c r="AF5" s="88"/>
+      <c r="AG5" s="88"/>
+      <c r="AH5" s="88"/>
+      <c r="AI5" s="88"/>
+      <c r="AJ5" s="89"/>
+      <c r="AK5" s="89"/>
+      <c r="AL5" s="89"/>
+      <c r="AM5" s="80"/>
+      <c r="AN5" s="80"/>
+      <c r="AO5" s="70"/>
+      <c r="AP5" s="70"/>
+      <c r="AQ5" s="70"/>
+      <c r="AR5" s="70"/>
+      <c r="AS5" s="71"/>
+      <c r="AT5" s="71"/>
+      <c r="AU5" s="71"/>
+      <c r="AV5" s="71"/>
+      <c r="AW5" s="71"/>
+      <c r="AX5" s="71"/>
+      <c r="AY5" s="71"/>
+      <c r="AZ5" s="71"/>
+      <c r="BA5" s="71"/>
+      <c r="BB5" s="71"/>
+      <c r="BC5" s="71"/>
+      <c r="BD5" s="71"/>
+      <c r="BE5" s="71"/>
+      <c r="BF5" s="71"/>
+      <c r="BG5" s="71"/>
+      <c r="BH5" s="71"/>
+      <c r="BI5" s="71"/>
+      <c r="BJ5" s="71"/>
       <c r="BK5" s="8" t="s">
         <v>27</v>
       </c>
@@ -4463,38 +4471,38 @@
       <c r="JL5" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="JM5" s="89"/>
-      <c r="JN5" s="89"/>
-      <c r="JO5" s="89"/>
-      <c r="JP5" s="89"/>
-      <c r="JQ5" s="89"/>
-      <c r="JR5" s="89"/>
-      <c r="JS5" s="89"/>
-      <c r="JT5" s="89"/>
-      <c r="JU5" s="89"/>
-      <c r="JV5" s="89"/>
-      <c r="JW5" s="89"/>
-      <c r="JX5" s="89"/>
-      <c r="JY5" s="89"/>
-      <c r="JZ5" s="87" t="s">
+      <c r="JM5" s="69"/>
+      <c r="JN5" s="69"/>
+      <c r="JO5" s="69"/>
+      <c r="JP5" s="69"/>
+      <c r="JQ5" s="69"/>
+      <c r="JR5" s="69"/>
+      <c r="JS5" s="69"/>
+      <c r="JT5" s="69"/>
+      <c r="JU5" s="69"/>
+      <c r="JV5" s="69"/>
+      <c r="JW5" s="69"/>
+      <c r="JX5" s="69"/>
+      <c r="JY5" s="69"/>
+      <c r="JZ5" s="66" t="s">
         <v>316</v>
       </c>
-      <c r="KA5" s="87"/>
-      <c r="KB5" s="87"/>
-      <c r="KC5" s="87"/>
-      <c r="KD5" s="87" t="s">
+      <c r="KA5" s="66"/>
+      <c r="KB5" s="66"/>
+      <c r="KC5" s="66"/>
+      <c r="KD5" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="KE5" s="87"/>
-      <c r="KF5" s="87"/>
-      <c r="KG5" s="87"/>
-      <c r="KH5" s="84"/>
-      <c r="KI5" s="85"/>
-      <c r="KJ5" s="85"/>
-      <c r="KK5" s="85"/>
+      <c r="KE5" s="66"/>
+      <c r="KF5" s="66"/>
+      <c r="KG5" s="66"/>
+      <c r="KH5" s="63"/>
+      <c r="KI5" s="64"/>
+      <c r="KJ5" s="64"/>
+      <c r="KK5" s="64"/>
       <c r="KL5" s="60"/>
     </row>
-    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:298" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -5390,7 +5398,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>343</v>
       </c>
@@ -6312,7 +6320,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="8" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>365</v>
       </c>
@@ -7234,7 +7242,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="9" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>378</v>
       </c>
@@ -8156,7 +8164,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="10" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>397</v>
       </c>
@@ -9078,7 +9086,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="11" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:298" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>408</v>
       </c>
@@ -10001,22 +10009,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:KK6">
-    <sortState ref="A7:KK10">
+  <autoFilter ref="A6:KK6" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:KK10">
       <sortCondition ref="KK6"/>
     </sortState>
   </autoFilter>
   <mergeCells count="32">
-    <mergeCell ref="KH4:KK5"/>
-    <mergeCell ref="JZ4:KG4"/>
-    <mergeCell ref="JZ5:KC5"/>
-    <mergeCell ref="KD5:KG5"/>
-    <mergeCell ref="GU4:HH4"/>
-    <mergeCell ref="HI4:HV4"/>
-    <mergeCell ref="HW4:IJ4"/>
-    <mergeCell ref="IK4:IX4"/>
-    <mergeCell ref="IY4:JL4"/>
-    <mergeCell ref="JM4:JY5"/>
+    <mergeCell ref="AM4:AN5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A4:D5"/>
+    <mergeCell ref="E4:J5"/>
+    <mergeCell ref="K4:O5"/>
+    <mergeCell ref="P4:T5"/>
+    <mergeCell ref="U4:AB5"/>
+    <mergeCell ref="AC4:AI5"/>
+    <mergeCell ref="AJ4:AL5"/>
     <mergeCell ref="GG4:GT4"/>
     <mergeCell ref="AO4:AR5"/>
     <mergeCell ref="AS4:BJ5"/>
@@ -10029,31 +10037,31 @@
     <mergeCell ref="EQ4:FD4"/>
     <mergeCell ref="FE4:FR4"/>
     <mergeCell ref="FS4:GF4"/>
-    <mergeCell ref="AM4:AN5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A4:D5"/>
-    <mergeCell ref="E4:J5"/>
-    <mergeCell ref="K4:O5"/>
-    <mergeCell ref="P4:T5"/>
-    <mergeCell ref="U4:AB5"/>
-    <mergeCell ref="AC4:AI5"/>
-    <mergeCell ref="AJ4:AL5"/>
+    <mergeCell ref="KH4:KK5"/>
+    <mergeCell ref="JZ4:KG4"/>
+    <mergeCell ref="JZ5:KC5"/>
+    <mergeCell ref="KD5:KG5"/>
+    <mergeCell ref="GU4:HH4"/>
+    <mergeCell ref="HI4:HV4"/>
+    <mergeCell ref="HW4:IJ4"/>
+    <mergeCell ref="IK4:IX4"/>
+    <mergeCell ref="IY4:JL4"/>
+    <mergeCell ref="JM4:JY5"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A6">
     <cfRule type="duplicateValues" dxfId="0" priority="92"/>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="4">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR11">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP1:AR3 AO1:AO4 AO7:AR11" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>36526</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7:KI11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KI7:KI11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete, No Delivery pre 2021 "</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7:KK11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KK7:KK11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"NGSA, WEM, FCRM Operational Framework, Other, Unknown/TBC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7:KH11 KJ7:KJ11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="KH7:KH11 KJ7:KJ11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"4. High, 3. Medium High, 2. Medium Low, 1. Low, Already Complete,"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10061,4 +10069,16 @@
   <pageSetup paperSize="9" scale="10" orientation="landscape"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BBB8C6-3FA0-4446-A91C-24D37E1D0F94}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>